<commit_message>
Merged excel and gigachad
</commit_message>
<xml_diff>
--- a/Habitat_Design_Specification.xlsx
+++ b/Habitat_Design_Specification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="10452" yWindow="1728" windowWidth="14340" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Design Specification" sheetId="1" state="visible" r:id="rId1"/>
@@ -225,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -262,8 +262,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +689,8 @@
   </sheetPr>
   <dimension ref="A3:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -724,17 +722,17 @@
       <c r="P3" s="25" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="26" t="inlineStr">
+      <c r="A4" s="14" t="inlineStr">
         <is>
           <t>Geometric outline</t>
         </is>
       </c>
-      <c r="B4" s="27" t="inlineStr">
+      <c r="B4" s="15" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="C4" s="27" t="inlineStr">
+      <c r="C4" s="15" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
@@ -759,7 +757,7 @@
         </is>
       </c>
       <c r="B5" s="16" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="C5" s="17" t="inlineStr">
         <is>
@@ -779,12 +777,12 @@
       <c r="P5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="27" t="inlineStr">
+      <c r="A6" s="15" t="inlineStr">
         <is>
           <t>Floors</t>
         </is>
       </c>
-      <c r="B6" s="27" t="n">
+      <c r="B6" s="15" t="n">
         <v>0.07000000000000001</v>
       </c>
       <c r="C6" s="19" t="inlineStr">
@@ -833,12 +831,12 @@
       <c r="P7" s="11" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="inlineStr">
+      <c r="A8" s="15" t="inlineStr">
         <is>
           <t>Base diameter</t>
         </is>
       </c>
-      <c r="B8" s="27" t="n"/>
+      <c r="B8" s="15" t="n"/>
       <c r="C8" s="19" t="inlineStr">
         <is>
           <t>[]</t>
@@ -904,8 +902,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="27" t="n"/>
-      <c r="B12" s="27" t="n"/>
+      <c r="A12" s="15" t="n"/>
+      <c r="B12" s="15" t="n"/>
       <c r="C12" s="19" t="inlineStr">
         <is>
           <t>[kW]</t>
@@ -922,8 +920,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="27" t="n"/>
-      <c r="B14" s="27" t="n"/>
+      <c r="A14" s="15" t="n"/>
+      <c r="B14" s="15" t="n"/>
       <c r="C14" s="19" t="inlineStr">
         <is>
           <t>[kW]</t>
@@ -940,8 +938,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="26" t="n"/>
-      <c r="B16" s="27" t="n"/>
+      <c r="A16" s="14" t="n"/>
+      <c r="B16" s="15" t="n"/>
       <c r="C16" s="19" t="inlineStr">
         <is>
           <t>[kW]</t>
@@ -962,13 +960,13 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="26" t="inlineStr">
+      <c r="A18" s="14" t="inlineStr">
         <is>
           <t>Heating/Radiator</t>
         </is>
       </c>
-      <c r="B18" s="27" t="n">
-        <v>-0.903677782860531</v>
+      <c r="B18" s="15" t="n">
+        <v>0.1009602692747351</v>
       </c>
       <c r="C18" s="19" t="inlineStr">
         <is>
@@ -999,12 +997,12 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="inlineStr">
+      <c r="A21" s="15" t="inlineStr">
         <is>
           <t>Lifesupport</t>
         </is>
       </c>
-      <c r="B21" s="27" t="n">
+      <c r="B21" s="15" t="n">
         <v>50</v>
       </c>
       <c r="C21" s="19" t="inlineStr">
@@ -1029,12 +1027,12 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="27" t="inlineStr">
+      <c r="A23" s="15" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
-      <c r="B23" s="27" t="n">
+      <c r="B23" s="15" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="19" t="inlineStr">
@@ -1059,8 +1057,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="27" t="n"/>
-      <c r="B25" s="27" t="n">
+      <c r="A25" s="15" t="n"/>
+      <c r="B25" s="15" t="n">
         <v>52</v>
       </c>
       <c r="C25" s="19" t="inlineStr">

</xml_diff>